<commit_message>
Configuration Stage 1: Jan 6
</commit_message>
<xml_diff>
--- a/Daily Streak.xlsx
+++ b/Daily Streak.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\PractiseDSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07289A8-1BA9-49A2-8B8E-1B397DEE8914}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7426A4EC-CCB4-48BE-A9AF-D9164AFF2F94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7545" xr2:uid="{2FB7B406-D07E-4C18-88FC-8740F8091689}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>stack</t>
   </si>
@@ -109,12 +110,51 @@
   </si>
   <si>
     <t>geometry</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Day 1</t>
+  </si>
+  <si>
+    <t>Day 3</t>
+  </si>
+  <si>
+    <t>Day 5</t>
+  </si>
+  <si>
+    <t>Day 7</t>
+  </si>
+  <si>
+    <t>Stage 1: First Study</t>
+  </si>
+  <si>
+    <t>Stage 2: Review 1 + 2 + 3</t>
+  </si>
+  <si>
+    <t>Stage 3: Practise</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>1+ Month(s)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-1010409]d\ mmmm\ yyyy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -124,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,6 +174,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -159,6 +205,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B7EEDC-2C4B-4962-A07D-B56EFD341E4B}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,9 +543,10 @@
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -500,8 +559,11 @@
       <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -512,7 +574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -523,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -534,7 +596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -545,7 +607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -556,18 +618,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E7" s="5">
+        <v>45663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -578,18 +643,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>45663</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -602,61 +670,68 @@
       <c r="D10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="E10" s="5">
+        <v>45664</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B11" s="7">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B12" s="7">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="B13" s="7">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="B14" s="7">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -666,8 +741,11 @@
       <c r="C15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="5">
+        <v>45664</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -677,8 +755,11 @@
       <c r="C16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="5">
+        <v>45664</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -688,8 +769,11 @@
       <c r="C17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="5">
+        <v>45664</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -703,7 +787,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -714,7 +798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -723,4 +807,75 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480BB9B5-2EB6-400E-B6A7-267D86053734}">
+  <dimension ref="A2:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Stage 1: Jan 7
</commit_message>
<xml_diff>
--- a/Daily Streak.xlsx
+++ b/Daily Streak.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\PractiseDSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7426A4EC-CCB4-48BE-A9AF-D9164AFF2F94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477B7DD4-E539-4D34-B92E-31FA7262817A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7545" xr2:uid="{2FB7B406-D07E-4C18-88FC-8740F8091689}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>stack</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>1+ Month(s)</t>
+  </si>
+  <si>
+    <t>intermediate dp</t>
   </si>
 </sst>
 </file>
@@ -196,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -214,6 +217,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -531,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B7EEDC-2C4B-4962-A07D-B56EFD341E4B}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,6 +579,9 @@
       <c r="C2" s="2">
         <v>0</v>
       </c>
+      <c r="E2" s="5">
+        <v>45665</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -584,6 +593,9 @@
       <c r="C3" s="2">
         <v>0</v>
       </c>
+      <c r="E3" s="5">
+        <v>45665</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -595,6 +607,9 @@
       <c r="C4" s="1">
         <v>0</v>
       </c>
+      <c r="E4" s="5">
+        <v>45665</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -606,6 +621,9 @@
       <c r="C5" s="1">
         <v>0</v>
       </c>
+      <c r="E5" s="5">
+        <v>45665</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -665,7 +683,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
@@ -742,7 +760,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="5">
-        <v>45664</v>
+        <v>45665</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -756,10 +774,10 @@
         <v>0</v>
       </c>
       <c r="E16" s="5">
-        <v>45664</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45665</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -769,11 +787,8 @@
       <c r="C17" s="1">
         <v>0</v>
       </c>
-      <c r="E17" s="5">
-        <v>45664</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -787,7 +802,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -798,9 +813,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -814,7 +846,7 @@
   <dimension ref="A2:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,17 +865,17 @@
       <c r="A2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
Stage 1: Jan 9
</commit_message>
<xml_diff>
--- a/Daily Streak.xlsx
+++ b/Daily Streak.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\PractiseDSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477B7DD4-E539-4D34-B92E-31FA7262817A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419CBA15-AA8C-436A-ABF4-325EAA7301B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7545" xr2:uid="{2FB7B406-D07E-4C18-88FC-8740F8091689}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>stack</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>intermediate dp</t>
+  </si>
+  <si>
+    <t>topo sort</t>
   </si>
 </sst>
 </file>
@@ -167,7 +170,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +189,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -199,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -223,6 +232,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B7EEDC-2C4B-4962-A07D-B56EFD341E4B}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,9 +597,6 @@
       <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="E2" s="5">
-        <v>45665</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -593,22 +608,19 @@
       <c r="C3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="5">
-        <v>45665</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4" s="5">
-        <v>45665</v>
+        <v>45666</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -621,9 +633,6 @@
       <c r="C5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="5">
-        <v>45665</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -680,7 +689,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1">
         <v>4</v>
@@ -750,88 +759,97 @@
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="12">
+        <v>0</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="5">
-        <v>45665</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B16" s="14">
+        <v>0</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0</v>
+      </c>
+      <c r="E16" s="15"/>
+    </row>
+    <row r="17" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="5">
-        <v>45665</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" s="14">
+        <v>0</v>
+      </c>
+      <c r="C17" s="14">
+        <v>0</v>
+      </c>
+      <c r="E17" s="15">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="9">
-        <v>0</v>
-      </c>
-      <c r="C20" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21" s="9">
+        <v>0</v>
+      </c>
+      <c r="C21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="9">
-        <v>0</v>
-      </c>
-      <c r="C21" s="9">
+      <c r="B22" s="9">
+        <v>0</v>
+      </c>
+      <c r="C22" s="9">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Configuration Files & Folders
</commit_message>
<xml_diff>
--- a/Daily Streak.xlsx
+++ b/Daily Streak.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\PractiseDSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419CBA15-AA8C-436A-ABF4-325EAA7301B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDD815A-4DB2-407D-9405-3320368C45AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7545" xr2:uid="{2FB7B406-D07E-4C18-88FC-8740F8091689}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>stack</t>
   </si>
@@ -113,39 +112,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>Day 1</t>
-  </si>
-  <si>
-    <t>Day 3</t>
-  </si>
-  <si>
-    <t>Day 5</t>
-  </si>
-  <si>
-    <t>Day 7</t>
-  </si>
-  <si>
-    <t>Stage 1: First Study</t>
-  </si>
-  <si>
-    <t>Stage 2: Review 1 + 2 + 3</t>
-  </si>
-  <si>
-    <t>Stage 3: Practise</t>
-  </si>
-  <si>
-    <t>Week 2</t>
-  </si>
-  <si>
-    <t>Week 3</t>
-  </si>
-  <si>
-    <t>Week 4</t>
-  </si>
-  <si>
-    <t>1+ Month(s)</t>
   </si>
   <si>
     <t>intermediate dp</t>
@@ -208,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -226,9 +192,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -558,7 +521,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +530,7 @@
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -759,39 +722,41 @@
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="12">
-        <v>0</v>
-      </c>
-      <c r="C15" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="11">
+        <v>0</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="14">
-        <v>0</v>
-      </c>
-      <c r="C16" s="14">
-        <v>0</v>
-      </c>
-      <c r="E16" s="15"/>
-    </row>
-    <row r="17" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="B16" s="13">
+        <v>0</v>
+      </c>
+      <c r="C16" s="13">
+        <v>0</v>
+      </c>
+      <c r="E16" s="14">
+        <v>45667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="14">
-        <v>0</v>
-      </c>
-      <c r="C17" s="14">
-        <v>0</v>
-      </c>
-      <c r="E17" s="15">
+      <c r="B17" s="13">
+        <v>0</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0</v>
+      </c>
+      <c r="E17" s="14">
         <v>45666</v>
       </c>
     </row>
@@ -819,6 +784,9 @@
       <c r="D19" t="s">
         <v>25</v>
       </c>
+      <c r="E19" s="5">
+        <v>45667</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -844,7 +812,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B22" s="9">
         <v>0</v>
@@ -857,75 +825,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{480BB9B5-2EB6-400E-B6A7-267D86053734}">
-  <dimension ref="A2:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:H2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>